<commit_message>
No Hopeless Romance 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/No Hopeless Romance - 2964282061/No Hopeless Romance - 2964282061.xlsx
+++ b/Data/No Hopeless Romance - 2964282061/No Hopeless Romance - 2964282061.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\No Hopeless Romance - 2964282061\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD132F6-C9D1-4F87-9B51-F2550D30F121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F0EB91-D09A-44CC-8CC6-5F1F15040B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -218,10 +218,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>호환성 임계값:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>궁합은 폰이 서로 상호작용하는 방식을 판단하는 숨겨진 가치입니다. 궁합이 낮으면 모욕과 무시를 더 많이 합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -284,6 +280,29 @@
   <si>
     <t>Should A has no spouse</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No more mutual reject.</t>
+  </si>
+  <si>
+    <t>NHR.Consensus</t>
+  </si>
+  <si>
+    <t>NHR.Consensus_Tip</t>
+  </si>
+  <si>
+    <t>궁합 임계값:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>더 이상 상호 거부가 없습니다.</t>
+  </si>
+  <si>
+    <t>Consensus romance always succeed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>합의된 로맨스는 언제나 성공합니다</t>
   </si>
 </sst>
 </file>
@@ -635,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -685,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -750,10 +769,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -767,10 +786,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -787,7 +806,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -804,7 +823,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -838,7 +857,7 @@
         <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -852,10 +871,10 @@
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -872,7 +891,7 @@
         <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -889,7 +908,7 @@
         <v>42</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -906,7 +925,7 @@
         <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -923,7 +942,7 @@
         <v>48</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -940,7 +959,7 @@
         <v>51</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,7 +976,7 @@
         <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -974,7 +993,7 @@
         <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -991,7 +1010,35 @@
         <v>60</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>